<commit_message>
added summary section and calculations
</commit_message>
<xml_diff>
--- a/PlanetDollarSizing.xlsx
+++ b/PlanetDollarSizing.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graboskyc/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graboskyc/Documents/GitHub/MongoDBSizing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{3ED47FA5-EDE3-EE4F-A0CA-A5F7410B0F72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EB89E7-2418-9348-B1E4-F6AD41ECF787}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="1560" windowWidth="51200" windowHeight="21160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1560" windowWidth="51200" windowHeight="21160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sizing" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
   <si>
     <t>Assumptions</t>
   </si>
@@ -270,13 +269,16 @@
     <t>Estimated IOPS</t>
   </si>
   <si>
-    <t>Estimated shards needed</t>
-  </si>
-  <si>
     <t>Atlas max is 4TB</t>
   </si>
   <si>
     <t>Average Event Size (bytes)</t>
+  </si>
+  <si>
+    <t>Estimated shard count needed</t>
+  </si>
+  <si>
+    <t>Shard count's limiting factor is</t>
   </si>
 </sst>
 </file>
@@ -284,10 +286,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000E+00"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -334,6 +336,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -397,7 +405,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -426,14 +434,14 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyAlignment="1">
@@ -441,10 +449,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -762,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J99"/>
+  <dimension ref="A2:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="293" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="293" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1086,8 +1102,8 @@
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
-        <v>82</v>
+      <c r="A24" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="B24" s="11">
         <v>1024</v>
@@ -1795,7 +1811,7 @@
       <c r="A68" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="25">
+      <c r="B68" s="24">
         <f>B32*60</f>
         <v>300000</v>
       </c>
@@ -1812,7 +1828,7 @@
       <c r="A69" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="25">
+      <c r="B69" s="24">
         <f>B31/60</f>
         <v>1.6666666666666667</v>
       </c>
@@ -1829,7 +1845,7 @@
       <c r="A70" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B70" s="25">
+      <c r="B70" s="24">
         <f>B69*B68</f>
         <v>500000</v>
       </c>
@@ -1848,7 +1864,7 @@
       <c r="A71" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B71" s="25">
+      <c r="B71" s="24">
         <f>B70*(1-B26)</f>
         <v>49999.999999999985</v>
       </c>
@@ -1986,8 +2002,8 @@
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
-      <c r="G80" s="24" t="s">
-        <v>81</v>
+      <c r="G80" s="23" t="s">
+        <v>80</v>
       </c>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
@@ -2057,7 +2073,10 @@
         <f>ROUNDUP(C50/B79,0)</f>
         <v>1</v>
       </c>
-      <c r="C85" s="4"/>
+      <c r="C85" s="25" t="str">
+        <f>A85</f>
+        <v>Based on RAM</v>
+      </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
@@ -2074,7 +2093,10 @@
         <f>ROUNDUP((C38+C43)/B80,0)</f>
         <v>7</v>
       </c>
-      <c r="C86" s="4"/>
+      <c r="C86" s="25" t="str">
+        <f t="shared" ref="C86:C87" si="5">A86</f>
+        <v>Based on Disk Space</v>
+      </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -2088,9 +2110,13 @@
         <v>69</v>
       </c>
       <c r="B87" s="7">
+        <f>ROUNDUP(B73/B81,0)</f>
         <v>9</v>
       </c>
-      <c r="C87" s="4"/>
+      <c r="C87" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>Based on IOPS</v>
+      </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
@@ -2112,7 +2138,7 @@
       <c r="J88" s="4"/>
     </row>
     <row r="89" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="23" t="s">
         <v>70</v>
       </c>
       <c r="B89" s="15">
@@ -2147,7 +2173,7 @@
       <c r="A95" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B95" s="23">
+      <c r="B95" s="26">
         <f>D38</f>
         <v>70.243701338768005</v>
       </c>
@@ -2156,7 +2182,7 @@
       <c r="A96" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B96" s="23">
+      <c r="B96" s="26">
         <f>D43</f>
         <v>39.198494050651789</v>
       </c>
@@ -2165,7 +2191,7 @@
       <c r="A97" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B97" s="15">
+      <c r="B97" s="27">
         <f>C50</f>
         <v>14.021247625350952</v>
       </c>
@@ -2174,18 +2200,27 @@
       <c r="A98" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B98" s="15">
+      <c r="B98" s="27">
         <f>B73</f>
         <v>65049.999999999985</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="B99" s="15">
+        <v>82</v>
+      </c>
+      <c r="B99" s="27">
         <f>B89</f>
         <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B100" s="27" t="str">
+        <f>VLOOKUP(B89,B85:C87,2,TRUE)</f>
+        <v>Based on IOPS</v>
       </c>
     </row>
   </sheetData>

</xml_diff>